<commit_message>
Removed student grading from page 2
</commit_message>
<xml_diff>
--- a/LabStarters/Lab03/Lab3Rubric-CIS195_8wk.xlsx
+++ b/LabStarters/Lab03/Lab3Rubric-CIS195_8wk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7118A5FB-1DC3-4F4B-9F9C-63AF7B2E3DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E43A5C-96D6-4E98-891F-3398EE6A43D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="3300" windowWidth="14916" windowHeight="12972" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="516" yWindow="3300" windowWidth="14916" windowHeight="12972" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="17">
   <si>
     <t>Elements used:</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>Code quality</t>
-  </si>
-  <si>
-    <t>Indentation</t>
   </si>
 </sst>
 </file>
@@ -150,12 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:B20"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -608,10 +604,10 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <f>SUM(B11:B17)</f>
         <v>20</v>
       </c>
@@ -640,10 +636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection sqref="A1:D20"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -654,12 +650,12 @@
     <col min="4" max="4" width="21.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -670,7 +666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -681,7 +677,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -692,7 +688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -703,7 +699,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -714,7 +710,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -722,13 +718,10 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -738,15 +731,15 @@
       </c>
       <c r="C8">
         <f>SUM(C3:C7)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -757,7 +750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -768,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -779,7 +772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -790,7 +783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -801,7 +794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -824,14 +817,14 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18">
         <f>SUM(B11:B17)</f>
         <v>20</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18">
         <f>SUM(C11:C17)</f>
         <v>20</v>
       </c>
@@ -846,7 +839,7 @@
       </c>
       <c r="C20">
         <f>C8+C18</f>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>